<commit_message>
Update java version to java 17, fixes #3971
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/sample-file-append.xlsx
+++ b/integration-tests/spreadsheet/files/sample-file-append.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/git/hop/integration-tests/spreadsheet/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F7E64-1DB6-E248-9927-BAFDBF4D7745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>column1</t>
   </si>
@@ -76,12 +76,73 @@
   </si>
   <si>
     <t>here</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>dssdfd</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>gfdsgdfs</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>sfdgf</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>sdfgfsd</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>sdfgsfd</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>sfgsfg</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>fsdgdfs</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>sfgfsdfg</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>jj</t>
+  </si>
+  <si>
+    <t>sfgffd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,48 +513,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.33203125"/>
+    <col min="3" max="3" customWidth="true" width="13.5"/>
+    <col min="4" max="4" customWidth="true" width="18.5"/>
+    <col min="5" max="5" customWidth="true" width="15.6640625"/>
+    <col min="6" max="6" customWidth="true" width="20.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -501,10 +562,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -512,10 +573,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -523,10 +584,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -534,10 +595,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -545,10 +606,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -556,10 +617,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -567,14 +628,124 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -598,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
switch to java 17, fixes #3971 (#3972)
* Update java version to java 17, fixes #3971

* Update github actions java version

* update rat plugin
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/sample-file-append.xlsx
+++ b/integration-tests/spreadsheet/files/sample-file-append.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/git/hop/integration-tests/spreadsheet/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F7E64-1DB6-E248-9927-BAFDBF4D7745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>column1</t>
   </si>
@@ -76,12 +76,73 @@
   </si>
   <si>
     <t>here</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>dssdfd</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>gfdsgdfs</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>sfdgf</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>sdfgfsd</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>sdfgsfd</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>sfgsfg</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>fsdgdfs</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>sfgfsdfg</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>jj</t>
+  </si>
+  <si>
+    <t>sfgffd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,48 +513,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.33203125"/>
+    <col min="3" max="3" customWidth="true" width="13.5"/>
+    <col min="4" max="4" customWidth="true" width="18.5"/>
+    <col min="5" max="5" customWidth="true" width="15.6640625"/>
+    <col min="6" max="6" customWidth="true" width="20.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -501,10 +562,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -512,10 +573,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -523,10 +584,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -534,10 +595,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -545,10 +606,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -556,10 +617,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -567,14 +628,124 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -598,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
fix some test , #4036
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/sample-file-append.xlsx
+++ b/integration-tests/spreadsheet/files/sample-file-append.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10602"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/git/hop/integration-tests/spreadsheet/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F7E64-1DB6-E248-9927-BAFDBF4D7745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CA716-8987-3E4F-96C1-FF0DFFC13541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="47920" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>column1</t>
   </si>
@@ -76,73 +76,12 @@
   </si>
   <si>
     <t>here</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>dssdfd</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>gfdsgdfs</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>sfdgf</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>sdfgfsd</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>sdfgsfd</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>sfgsfg</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>fsdgdfs</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>sfgfsdfg</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
-    <t>sdfg</t>
-  </si>
-  <si>
-    <t>jj</t>
-  </si>
-  <si>
-    <t>sfgffd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,9 +132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,9 +172,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,26 +207,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,26 +242,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,48 +418,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.33203125"/>
-    <col min="3" max="3" customWidth="true" width="13.5"/>
-    <col min="4" max="4" customWidth="true" width="18.5"/>
-    <col min="5" max="5" customWidth="true" width="15.6640625"/>
-    <col min="6" max="6" customWidth="true" width="20.33203125"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -562,10 +467,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -573,10 +478,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -584,10 +489,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -595,10 +500,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -606,10 +511,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -617,10 +522,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -628,124 +533,14 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -769,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
fix some Java 17 things and disable flink, fixes #4036 (#4037)
* fix some test , #4036

* fix some more java issues, #4036

* remove nashorn, invalid license, fixes #4036
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/sample-file-append.xlsx
+++ b/integration-tests/spreadsheet/files/sample-file-append.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10602"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/git/hop/integration-tests/spreadsheet/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F7E64-1DB6-E248-9927-BAFDBF4D7745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CA716-8987-3E4F-96C1-FF0DFFC13541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49520" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="47920" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>column1</t>
   </si>
@@ -76,73 +76,12 @@
   </si>
   <si>
     <t>here</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>dssdfd</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>gfdsgdfs</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>sfdgf</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>sdfgfsd</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>sdfgsfd</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>sfgsfg</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>fsdgdfs</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>sfgfsdfg</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
-    <t>sdfg</t>
-  </si>
-  <si>
-    <t>jj</t>
-  </si>
-  <si>
-    <t>sfgffd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,9 +132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,9 +172,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,26 +207,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,26 +242,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,48 +418,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.33203125"/>
-    <col min="3" max="3" customWidth="true" width="13.5"/>
-    <col min="4" max="4" customWidth="true" width="18.5"/>
-    <col min="5" max="5" customWidth="true" width="15.6640625"/>
-    <col min="6" max="6" customWidth="true" width="20.33203125"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -562,10 +467,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -573,10 +478,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -584,10 +489,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -595,10 +500,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -606,10 +511,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -617,10 +522,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -628,124 +533,14 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -769,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Move assembly pom to plugin, fixes #4102
fix version reference in pom

Cleanup Assemblies

Update assembly xsd version

fix assembly headers
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/sample-file-append.xlsx
+++ b/integration-tests/spreadsheet/files/sample-file-append.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/git/hop/integration-tests/spreadsheet/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CA716-8987-3E4F-96C1-FF0DFFC13541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAD0124-C486-DE4A-B185-75A9CD68C54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47920" yWindow="3960" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24920" yWindow="3780" windowWidth="20880" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD20"/>
+      <selection activeCell="D13" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>